<commit_message>
Implement Parquet file format for all v1.0.0 Save to Workspace
</commit_message>
<xml_diff>
--- a/src/mediaplanpy/excel/templates/default_template.xlsx
+++ b/src/mediaplanpy/excel/templates/default_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\PycharmProjects\mediaplanpy\src\mediaplanpy\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53625559-4ED7-46D6-B738-2C5DC729763F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184D24FE-9EEB-40B2-8C2F-658AF92CEAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{A49F2509-323B-4CCA-AD03-8F21AA3D8AA2}"/>
   </bookViews>
@@ -59,10 +59,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,8 +101,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,25 +468,29 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>